<commit_message>
input from keyboard for each type of run
</commit_message>
<xml_diff>
--- a/OptionalSubjectsRepartition/RepartizareRezultate/Formular opționale (răspunsuri).xlsx
+++ b/OptionalSubjectsRepartition/RepartizareRezultate/Formular opționale (răspunsuri).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\my_github\uipath\proiect_rpa\OptionalSubjectsRepartition\RepartizareRezultate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB59755-CCCE-4B32-9740-0F5219D024E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CD486E-B546-4F12-980F-3D544C69FB98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="945" yWindow="690" windowWidth="23070" windowHeight="10965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -382,7 +382,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8766DAA-DBC9-43C9-89FE-80602E592761}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4778AFB0-5366-4714-9D0F-D29C0951C0FE}">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -468,7 +468,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63720C5D-2F5F-462D-AF63-FA8276C3B2DB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B92E8203-0711-477E-AC17-65DEF34F8AFB}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -488,7 +488,7 @@
         <v>15</v>
       </c>
       <c r="B2">
-        <v>8.7899999999999991</v>
+        <v>7.54</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -496,7 +496,7 @@
         <v>16</v>
       </c>
       <c r="B3">
-        <v>8.1</v>
+        <v>6.5659999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -618,7 +618,7 @@
         <v>2</v>
       </c>
       <c r="P2">
-        <v>8.7899999999999991</v>
+        <v>7.54</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
@@ -668,7 +668,7 @@
         <v>1</v>
       </c>
       <c r="P3">
-        <v>8.1</v>
+        <v>6.5659999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>